<commit_message>
added gradle and other admin
</commit_message>
<xml_diff>
--- a/Kata1/TruthTable.xlsx
+++ b/Kata1/TruthTable.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\TDDKatas\Kata1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="0" windowWidth="17790" windowHeight="5430"/>
+    <workbookView xWindow="1320" yWindow="0" windowWidth="20040" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,19 +66,45 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -106,19 +128,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -396,92 +426,94 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="b">
+      <c r="E3" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="b">
+      <c r="E4" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>0</v>
       </c>
-      <c r="E5" t="b">
+      <c r="E5" s="5" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>